<commit_message>
edit Division_Yearb file to report each Year season
</commit_message>
<xml_diff>
--- a/Data/County_Division/Cleaned Data/Division_Year.xlsx
+++ b/Data/County_Division/Cleaned Data/Division_Year.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,6 +365,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Season</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Division_Year</t>
         </is>
       </c>
@@ -375,157 +380,897 @@
           <t>84</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C2">
         <v>82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>85</t>
-        </is>
-      </c>
-      <c r="B3">
+          <t>84</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C3">
         <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>86</t>
-        </is>
-      </c>
-      <c r="B4">
+          <t>84</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C4">
         <v>82</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>87</t>
-        </is>
-      </c>
-      <c r="B5">
+          <t>84</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C5">
         <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>88</t>
-        </is>
-      </c>
-      <c r="B6">
-        <v>85</v>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>89</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>85</v>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>89</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>88</v>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>90</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>91</v>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="B10">
-        <v>91</v>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>92</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>91</v>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>91</v>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>82</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>94</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>91</v>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>95</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>91</v>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>96</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>91</v>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>82</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="B16">
-        <v>92</v>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>82</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C56">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C57">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>98</t>
         </is>
       </c>
-      <c r="B17">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C58">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C59">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C60">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="C61">
         <v>92</v>
       </c>
     </row>

</xml_diff>